<commit_message>
Data Entry Added (Almost)
</commit_message>
<xml_diff>
--- a/TravelAway/Infosys.TravelAway/Infosys.TravelAway.DAL/TravelAwayDBSchema.xlsx
+++ b/TravelAway/Infosys.TravelAway/Infosys.TravelAway.DAL/TravelAwayDBSchema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\areetra.halder\source\repos\JUL22SET1NCSMSCOMPREAGROUP14\TravelAway\Infosys.TravelAway\Infosys.TravelAway.DAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31884BC1-B70A-44CB-B997-A866AF8C6572}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34EE528-0E84-4CEE-A874-45F2E5E21B0B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{F9715CF6-EB02-4350-8D86-EAD0EE4EECC9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Customer Table</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>Address</t>
+  </si>
+  <si>
+    <t>PackageID</t>
+  </si>
+  <si>
+    <t>Null</t>
   </si>
 </sst>
 </file>
@@ -403,13 +409,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87379E3D-8DFD-441C-85A5-930459AAD516}">
-  <dimension ref="B7:B16"/>
+  <dimension ref="B7:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -456,6 +465,14 @@
         <v>8</v>
       </c>
     </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>